<commit_message>
Update Journal de bord, Journal de travail + Add Maquette.png
</commit_message>
<xml_diff>
--- a/Informations/Journal de bord.xlsx
+++ b/Informations/Journal de bord.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Bataille\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bataille-Navale\Informations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92F052F-9EE2-4358-8541-AC90435DF11E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="5100" yWindow="2415" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>ICT 431</t>
   </si>
@@ -72,12 +73,18 @@
   </si>
   <si>
     <t>Création des scénarios de la bataille navale</t>
+  </si>
+  <si>
+    <t>Création de la maquette</t>
+  </si>
+  <si>
+    <t>Création de maquette</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -334,70 +341,70 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -679,11 +686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,212 +702,224 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>43874</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="18">
         <v>0.62152777777777801</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>43874</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.66319444444444442</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>43896</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.60972222222222217</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8">
+        <v>43896</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.99444444444444446</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Journal de travail - Update 11.03.20
</commit_message>
<xml_diff>
--- a/Informations/Journal de bord.xlsx
+++ b/Informations/Journal de bord.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bataille-Navale\Informations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel.MACHADO-PERE\Documents\GitHub\Bataille-Navale\Informations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92F052F-9EE2-4358-8541-AC90435DF11E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2415" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="2415" windowWidth="21600" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -686,11 +685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Création des redirections + Update Journal de bord & Journal de travail
</commit_message>
<xml_diff>
--- a/Informations/Journal de bord.xlsx
+++ b/Informations/Journal de bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>ICT 431</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Création de maquette</t>
+  </si>
+  <si>
+    <t>Création du Menu Principale</t>
+  </si>
+  <si>
+    <t>Créations du Menu Principale</t>
+  </si>
+  <si>
+    <t>Création de la redirection</t>
+  </si>
+  <si>
+    <t>Créations de la redirection</t>
   </si>
 </sst>
 </file>
@@ -689,7 +701,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,20 +829,44 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8">
+        <v>43902</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.70416666666666661</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8">
+        <v>43902</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.70416666666666661</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>

</xml_diff>

<commit_message>
Journal de bord & Journal de Travail - Update 14.03.20
</commit_message>
<xml_diff>
--- a/Informations/Journal de bord.xlsx
+++ b/Informations/Journal de bord.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel.MACHADO-PERE\Documents\GitHub\Bataille-Navale\Informations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bataille-Navale\Informations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4165554B-F71F-43A7-9521-9C7A747AA71C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2415" windowWidth="21600" windowHeight="11835"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>ICT 431</t>
   </si>
@@ -90,12 +91,18 @@
   </si>
   <si>
     <t>Créations de la redirection</t>
+  </si>
+  <si>
+    <t>Version 0.1 fini</t>
+  </si>
+  <si>
+    <t>Création de la version 0.1 terminé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -697,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,12 +876,24 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8">
+        <v>43904</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>

</xml_diff>